<commit_message>
add test cases in article module
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="281">
   <si>
     <t>Descreption</t>
   </si>
@@ -920,6 +920,55 @@
     <t xml:space="preserve">1- login as admin with vaild username and password 
 2- a request pages hould be  loaded with the appearance of table that inculde title,uploadedby , Date , satuts
 3-click on notificaton button </t>
+  </si>
+  <si>
+    <t>AM_10</t>
+  </si>
+  <si>
+    <t>AM_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the  article has been removed from article table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verfiy  when admin click  on accept or reject button  it should be removed from table article in the first request admin  page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- login as admin with vaild username and password 
+2- a request pages should be  loaded with the appearance of table that inculde uploaded by , title , Date , status button 
+3- click on Status Button
+4- a second request pages should be  loaded with the appearance of table that inculde uploaded by , title , Date , accept button , reject button
+5- click on accept or reject
+6-go back to first admin request page 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article should be removed from the table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article has been removed from article table in admin request page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- login as admin with vaild username and password 
+2- a request pages should be  loaded with the appearance of table that inculde uploaded by , title , Date , status button 
+3- click on Status Button
+4- a second request pages should be  loaded with the appearance of table that inculde uploaded by , title , Date , accept button , reject button
+5- click on accept or reject
+6-go back to first admin request page 
+7-open Database and see on tables articles that it has been added with new article
+</t>
+  </si>
+  <si>
+    <t>Article should be added in Database</t>
+  </si>
+  <si>
+    <t>Article is added in Database article table</t>
+  </si>
+  <si>
+    <t>Check that accpet article or reject article has been added in article tables in database</t>
+  </si>
+  <si>
+    <t>Verfiy when admin accpet or reject article in has been added in Data base</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1063,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1062,6 +1111,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1343,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA66"/>
+  <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1412,7 @@
     <col min="4" max="4" width="43.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="24.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="18" style="3" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" style="1" customWidth="1"/>
@@ -1374,7 +1429,7 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="10"/>
@@ -1994,7 +2049,7 @@
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="G27" s="19"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="13"/>
@@ -2607,7 +2662,7 @@
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
+      <c r="G56" s="19"/>
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
       <c r="J56" s="13"/>
@@ -2871,7 +2926,7 @@
       <c r="F66" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="G66" s="3"/>
+      <c r="G66" s="2"/>
       <c r="H66" s="6" t="s">
         <v>247</v>
       </c>
@@ -2883,6 +2938,64 @@
       </c>
       <c r="K66" s="1"/>
       <c r="L66" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="270" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="330" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="K68" s="1" t="s">
         <v>259</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Registration Module Test Cases have been added
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -1977,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="B57" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58:K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3270,7 +3270,7 @@
       <c r="J58" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L58" t="s">
+      <c r="K58" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3299,7 +3299,7 @@
       <c r="J59" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L59" t="s">
+      <c r="K59" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3328,7 +3328,7 @@
       <c r="J60" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L60" t="s">
+      <c r="K60" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       <c r="J61" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L61" t="s">
+      <c r="K61" t="s">
         <v>257</v>
       </c>
     </row>
@@ -3388,8 +3388,7 @@
       <c r="J62" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K62" s="6"/>
-      <c r="L62" s="7" t="s">
+      <c r="K62" s="7" t="s">
         <v>258</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2 test cases executed
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="410">
   <si>
     <t>Descreption</t>
   </si>
@@ -1548,12 +1548,21 @@
 6-Go to the databse
 7-Write a query to get the username just entered</t>
   </si>
+  <si>
+    <t>All the mentioned fields are present</t>
+  </si>
+  <si>
+    <t>There are no * beside the mandatory fields</t>
+  </si>
+  <si>
+    <t>Server error page comes up when pressing on submit button</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1598,7 +1607,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1614,6 +1623,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9797"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1654,7 +1675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1715,12 +1736,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9797"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1997,11 +2029,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B71" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G74" sqref="G73:G74"/>
+    <sheetView tabSelected="1" topLeftCell="C69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="32.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.453125" style="1" customWidth="1"/>
@@ -2014,10 +2046,10 @@
     <col min="9" max="9" width="18" style="3" customWidth="1"/>
     <col min="10" max="10" width="17.7265625" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.7265625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="4" customFormat="1" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" s="4" customFormat="1" ht="26.5" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
@@ -2031,8 +2063,9 @@
       <c r="I1" s="11"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="1:27" s="17" customFormat="1" ht="50.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:27" s="17" customFormat="1" ht="50.5" customHeight="1" thickBot="1">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
@@ -2066,7 +2099,7 @@
       <c r="K2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>256</v>
       </c>
       <c r="M2" s="16"/>
@@ -2085,7 +2118,7 @@
       <c r="Z2" s="16"/>
       <c r="AA2" s="16"/>
     </row>
-    <row r="3" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" ht="29">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -2108,7 +2141,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" ht="29">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -2131,7 +2164,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" ht="29">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -2154,7 +2187,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" ht="29">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -2177,7 +2210,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" ht="29">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -2200,7 +2233,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" ht="29">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2223,7 +2256,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" ht="29">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -2246,7 +2279,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" ht="47.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -2269,7 +2302,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" ht="43.5">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -2292,7 +2325,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" ht="29">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -2315,7 +2348,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" ht="43.5">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -2338,7 +2371,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" ht="43.5">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -2361,7 +2394,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="34.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" ht="34.15" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
@@ -2384,7 +2417,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" ht="43.5">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2407,7 +2440,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="43.5">
       <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
@@ -2430,7 +2463,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="29">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
@@ -2453,7 +2486,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="43.5">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -2476,7 +2509,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="29">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -2499,7 +2532,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="29">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -2522,7 +2555,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="43.5">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -2545,7 +2578,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="29">
       <c r="A23" s="1" t="s">
         <v>73</v>
       </c>
@@ -2568,7 +2601,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="29">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -2591,7 +2624,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="29">
       <c r="A25" s="1" t="s">
         <v>205</v>
       </c>
@@ -2614,7 +2647,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="29">
       <c r="A26" s="1" t="s">
         <v>206</v>
       </c>
@@ -2637,7 +2670,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="5" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" s="5" customFormat="1" ht="26">
       <c r="A27" s="12" t="s">
         <v>64</v>
       </c>
@@ -2651,8 +2684,9 @@
       <c r="I27" s="14"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
-    </row>
-    <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" ht="29">
       <c r="A28" s="1" t="s">
         <v>103</v>
       </c>
@@ -2675,7 +2709,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="30.65" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>104</v>
       </c>
@@ -2698,7 +2732,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="29">
       <c r="A30" s="1" t="s">
         <v>105</v>
       </c>
@@ -2721,7 +2755,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="29">
       <c r="A31" s="1" t="s">
         <v>106</v>
       </c>
@@ -2744,7 +2778,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="29">
       <c r="A32" s="1" t="s">
         <v>107</v>
       </c>
@@ -2767,7 +2801,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="43.5">
       <c r="A33" s="1" t="s">
         <v>108</v>
       </c>
@@ -2790,7 +2824,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="43.5">
       <c r="A34" s="1" t="s">
         <v>109</v>
       </c>
@@ -2813,7 +2847,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="58">
       <c r="A35" s="1" t="s">
         <v>110</v>
       </c>
@@ -2836,7 +2870,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="43.5">
       <c r="A36" s="1" t="s">
         <v>111</v>
       </c>
@@ -2859,7 +2893,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="43.5">
       <c r="A37" s="1" t="s">
         <v>112</v>
       </c>
@@ -2882,7 +2916,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="43.5">
       <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
@@ -2905,7 +2939,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="43.5">
       <c r="A39" s="1" t="s">
         <v>114</v>
       </c>
@@ -2928,7 +2962,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="43.5">
       <c r="A40" s="1" t="s">
         <v>115</v>
       </c>
@@ -2951,7 +2985,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="29">
       <c r="A41" s="1" t="s">
         <v>116</v>
       </c>
@@ -2974,7 +3008,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="27.65" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>117</v>
       </c>
@@ -2997,7 +3031,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="35.5" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>118</v>
       </c>
@@ -3020,7 +3054,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="29">
       <c r="A44" s="1" t="s">
         <v>119</v>
       </c>
@@ -3043,7 +3077,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="29">
       <c r="A45" s="1" t="s">
         <v>120</v>
       </c>
@@ -3066,7 +3100,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="29">
       <c r="A46" s="1" t="s">
         <v>121</v>
       </c>
@@ -3089,7 +3123,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="29">
       <c r="A47" s="1" t="s">
         <v>122</v>
       </c>
@@ -3112,7 +3146,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="29">
       <c r="A48" s="1" t="s">
         <v>123</v>
       </c>
@@ -3135,7 +3169,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" ht="29">
       <c r="A49" s="1" t="s">
         <v>124</v>
       </c>
@@ -3158,7 +3192,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" ht="29">
       <c r="A50" s="1" t="s">
         <v>125</v>
       </c>
@@ -3181,7 +3215,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" ht="29">
       <c r="A51" s="1" t="s">
         <v>126</v>
       </c>
@@ -3204,7 +3238,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" ht="29">
       <c r="A52" s="1" t="s">
         <v>127</v>
       </c>
@@ -3227,7 +3261,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" ht="29">
       <c r="A53" s="1" t="s">
         <v>128</v>
       </c>
@@ -3250,7 +3284,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:12" s="5" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" s="5" customFormat="1" ht="26">
       <c r="A56" s="12" t="s">
         <v>207</v>
       </c>
@@ -3264,8 +3298,9 @@
       <c r="I56" s="14"/>
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
-    </row>
-    <row r="58" spans="1:12" ht="135" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L56" s="13"/>
+    </row>
+    <row r="58" spans="1:12" ht="135" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>208</v>
       </c>
@@ -3294,11 +3329,11 @@
         <v>213</v>
       </c>
       <c r="K58"/>
-      <c r="L58" t="s">
+      <c r="L58" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="195" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" ht="195" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>214</v>
       </c>
@@ -3327,11 +3362,11 @@
         <v>213</v>
       </c>
       <c r="K59"/>
-      <c r="L59" t="s">
+      <c r="L59" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" ht="180" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>216</v>
       </c>
@@ -3360,11 +3395,11 @@
         <v>213</v>
       </c>
       <c r="K60"/>
-      <c r="L60" t="s">
+      <c r="L60" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="120" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" ht="120" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>222</v>
       </c>
@@ -3393,11 +3428,11 @@
         <v>213</v>
       </c>
       <c r="K61"/>
-      <c r="L61" t="s">
+      <c r="L61" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="7" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" s="7" customFormat="1" ht="105" customHeight="1">
       <c r="A62" s="6" t="s">
         <v>225</v>
       </c>
@@ -3426,11 +3461,11 @@
       <c r="J62" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L62" s="7" t="s">
+      <c r="L62" s="6" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="7" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" s="7" customFormat="1" ht="195" customHeight="1">
       <c r="A63" s="6" t="s">
         <v>228</v>
       </c>
@@ -3460,11 +3495,11 @@
         <v>213</v>
       </c>
       <c r="K63" s="6"/>
-      <c r="L63" s="7" t="s">
+      <c r="L63" s="6" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="7" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" s="7" customFormat="1" ht="195" customHeight="1">
       <c r="A64" s="6" t="s">
         <v>230</v>
       </c>
@@ -3494,11 +3529,11 @@
         <v>213</v>
       </c>
       <c r="K64" s="6"/>
-      <c r="L64" s="7" t="s">
+      <c r="L64" s="6" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="135" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" ht="135" customHeight="1">
       <c r="A65" s="6" t="s">
         <v>236</v>
       </c>
@@ -3526,11 +3561,11 @@
       <c r="J65" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L65" s="7" t="s">
+      <c r="L65" s="6" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="66" spans="1:12" s="8" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" s="8" customFormat="1" ht="225" customHeight="1">
       <c r="A66" s="1" t="s">
         <v>243</v>
       </c>
@@ -3560,11 +3595,11 @@
         <v>213</v>
       </c>
       <c r="K66" s="1"/>
-      <c r="L66" s="7" t="s">
+      <c r="L66" s="6" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="304.5">
       <c r="A67" s="1" t="s">
         <v>262</v>
       </c>
@@ -3596,7 +3631,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="348" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" ht="348">
       <c r="A68" s="1" t="s">
         <v>263</v>
       </c>
@@ -3628,7 +3663,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="5" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" s="5" customFormat="1" ht="26">
       <c r="A69" s="12" t="s">
         <v>372</v>
       </c>
@@ -3642,8 +3677,9 @@
       <c r="I69" s="14"/>
       <c r="J69" s="13"/>
       <c r="K69" s="13"/>
-    </row>
-    <row r="70" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="L69" s="13"/>
+    </row>
+    <row r="70" spans="1:12" ht="101.5">
       <c r="A70" s="6" t="s">
         <v>371</v>
       </c>
@@ -3666,14 +3702,18 @@
       <c r="H70" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="I70" s="20"/>
+      <c r="I70" s="20" t="s">
+        <v>407</v>
+      </c>
       <c r="J70" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K70" s="20"/>
-      <c r="L70" s="20"/>
-    </row>
-    <row r="71" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="L70" s="22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="72.5">
       <c r="A71" s="6" t="s">
         <v>373</v>
       </c>
@@ -3696,14 +3736,18 @@
       <c r="H71" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="I71" s="20"/>
+      <c r="I71" s="20" t="s">
+        <v>408</v>
+      </c>
       <c r="J71" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K71" s="20"/>
-      <c r="L71" s="20"/>
-    </row>
-    <row r="72" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="L71" s="23" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="101.5">
       <c r="A72" s="6" t="s">
         <v>374</v>
       </c>
@@ -3726,14 +3770,16 @@
       <c r="H72" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="I72" s="20"/>
+      <c r="I72" s="20" t="s">
+        <v>409</v>
+      </c>
       <c r="J72" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K72" s="20"/>
-      <c r="L72" s="20"/>
-    </row>
-    <row r="73" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="L72" s="6"/>
+    </row>
+    <row r="73" spans="1:12" ht="145">
       <c r="A73" s="6" t="s">
         <v>375</v>
       </c>
@@ -3761,9 +3807,9 @@
         <v>277</v>
       </c>
       <c r="K73" s="20"/>
-      <c r="L73" s="20"/>
-    </row>
-    <row r="74" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="L73" s="6"/>
+    </row>
+    <row r="74" spans="1:12" ht="116">
       <c r="A74" s="6" t="s">
         <v>376</v>
       </c>
@@ -3791,9 +3837,9 @@
         <v>277</v>
       </c>
       <c r="K74" s="20"/>
-      <c r="L74" s="20"/>
-    </row>
-    <row r="75" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="L74" s="6"/>
+    </row>
+    <row r="75" spans="1:12" ht="116">
       <c r="A75" s="6" t="s">
         <v>377</v>
       </c>
@@ -3821,9 +3867,9 @@
         <v>277</v>
       </c>
       <c r="K75" s="20"/>
-      <c r="L75" s="20"/>
-    </row>
-    <row r="76" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="L75" s="6"/>
+    </row>
+    <row r="76" spans="1:12" ht="116">
       <c r="A76" s="6" t="s">
         <v>378</v>
       </c>
@@ -3851,9 +3897,9 @@
         <v>277</v>
       </c>
       <c r="K76" s="20"/>
-      <c r="L76" s="20"/>
-    </row>
-    <row r="77" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="L76" s="6"/>
+    </row>
+    <row r="77" spans="1:12" ht="101.5">
       <c r="A77" s="6" t="s">
         <v>379</v>
       </c>
@@ -3881,9 +3927,9 @@
         <v>277</v>
       </c>
       <c r="K77" s="20"/>
-      <c r="L77" s="20"/>
-    </row>
-    <row r="78" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="L77" s="6"/>
+    </row>
+    <row r="78" spans="1:12" ht="116">
       <c r="A78" s="6" t="s">
         <v>380</v>
       </c>
@@ -3913,9 +3959,9 @@
         <v>277</v>
       </c>
       <c r="K78" s="20"/>
-      <c r="L78" s="20"/>
-    </row>
-    <row r="79" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+      <c r="L78" s="6"/>
+    </row>
+    <row r="79" spans="1:12" ht="87">
       <c r="A79" s="6" t="s">
         <v>381</v>
       </c>
@@ -3943,9 +3989,9 @@
       <c r="I79" s="20"/>
       <c r="J79" s="6"/>
       <c r="K79" s="20"/>
-      <c r="L79" s="20"/>
-    </row>
-    <row r="80" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="L79" s="6"/>
+    </row>
+    <row r="80" spans="1:12" ht="116">
       <c r="A80" s="6" t="s">
         <v>382</v>
       </c>
@@ -3975,9 +4021,9 @@
         <v>277</v>
       </c>
       <c r="K80" s="20"/>
-      <c r="L80" s="20"/>
-    </row>
-    <row r="81" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="L80" s="6"/>
+    </row>
+    <row r="81" spans="1:12" ht="101.5">
       <c r="A81" s="6" t="s">
         <v>383</v>
       </c>
@@ -4005,9 +4051,9 @@
         <v>277</v>
       </c>
       <c r="K81" s="20"/>
-      <c r="L81" s="20"/>
-    </row>
-    <row r="82" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="L81" s="6"/>
+    </row>
+    <row r="82" spans="1:12" ht="116">
       <c r="A82" s="6" t="s">
         <v>384</v>
       </c>
@@ -4035,9 +4081,9 @@
         <v>277</v>
       </c>
       <c r="K82" s="20"/>
-      <c r="L82" s="20"/>
-    </row>
-    <row r="83" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="L82" s="6"/>
+    </row>
+    <row r="83" spans="1:12" ht="145">
       <c r="A83" s="6" t="s">
         <v>385</v>
       </c>
@@ -4067,9 +4113,9 @@
         <v>277</v>
       </c>
       <c r="K83" s="20"/>
-      <c r="L83" s="20"/>
-    </row>
-    <row r="84" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="L83" s="6"/>
+    </row>
+    <row r="84" spans="1:12" ht="159.5">
       <c r="A84" s="6" t="s">
         <v>386</v>
       </c>
@@ -4099,9 +4145,9 @@
         <v>277</v>
       </c>
       <c r="K84" s="20"/>
-      <c r="L84" s="20"/>
-    </row>
-    <row r="85" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="L84" s="6"/>
+    </row>
+    <row r="85" spans="1:12" ht="159.5">
       <c r="A85" s="6" t="s">
         <v>387</v>
       </c>
@@ -4131,9 +4177,9 @@
         <v>277</v>
       </c>
       <c r="K85" s="20"/>
-      <c r="L85" s="20"/>
-    </row>
-    <row r="86" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="L85" s="6"/>
+    </row>
+    <row r="86" spans="1:12" ht="145">
       <c r="A86" s="6" t="s">
         <v>388</v>
       </c>
@@ -4163,9 +4209,9 @@
         <v>277</v>
       </c>
       <c r="K86" s="20"/>
-      <c r="L86" s="20"/>
-    </row>
-    <row r="87" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="L86" s="6"/>
+    </row>
+    <row r="87" spans="1:12" ht="159.5">
       <c r="A87" s="6" t="s">
         <v>389</v>
       </c>
@@ -4195,9 +4241,9 @@
         <v>277</v>
       </c>
       <c r="K87" s="20"/>
-      <c r="L87" s="20"/>
-    </row>
-    <row r="88" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="L87" s="6"/>
+    </row>
+    <row r="88" spans="1:12" ht="159.5">
       <c r="A88" s="6" t="s">
         <v>390</v>
       </c>
@@ -4227,9 +4273,9 @@
         <v>277</v>
       </c>
       <c r="K88" s="20"/>
-      <c r="L88" s="20"/>
-    </row>
-    <row r="89" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="L88" s="6"/>
+    </row>
+    <row r="89" spans="1:12" ht="145">
       <c r="A89" s="6" t="s">
         <v>391</v>
       </c>
@@ -4259,9 +4305,9 @@
         <v>277</v>
       </c>
       <c r="K89" s="20"/>
-      <c r="L89" s="20"/>
-    </row>
-    <row r="90" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="L89" s="6"/>
+    </row>
+    <row r="90" spans="1:12" ht="130.5">
       <c r="A90" s="6" t="s">
         <v>392</v>
       </c>
@@ -4291,9 +4337,9 @@
         <v>277</v>
       </c>
       <c r="K90" s="20"/>
-      <c r="L90" s="20"/>
-    </row>
-    <row r="91" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="L90" s="6"/>
+    </row>
+    <row r="91" spans="1:12" ht="145">
       <c r="A91" s="6" t="s">
         <v>393</v>
       </c>
@@ -4323,9 +4369,9 @@
         <v>277</v>
       </c>
       <c r="K91" s="20"/>
-      <c r="L91" s="20"/>
-    </row>
-    <row r="92" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="L91" s="6"/>
+    </row>
+    <row r="92" spans="1:12" ht="145">
       <c r="A92" s="6" t="s">
         <v>394</v>
       </c>
@@ -4355,9 +4401,9 @@
         <v>277</v>
       </c>
       <c r="K92" s="20"/>
-      <c r="L92" s="20"/>
-    </row>
-    <row r="93" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="L92" s="6"/>
+    </row>
+    <row r="93" spans="1:12" ht="145">
       <c r="A93" s="6" t="s">
         <v>395</v>
       </c>
@@ -4387,9 +4433,9 @@
         <v>277</v>
       </c>
       <c r="K93" s="20"/>
-      <c r="L93" s="20"/>
-    </row>
-    <row r="94" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+      <c r="L93" s="6"/>
+    </row>
+    <row r="94" spans="1:12" ht="145">
       <c r="A94" s="6" t="s">
         <v>396</v>
       </c>
@@ -4419,7 +4465,7 @@
         <v>277</v>
       </c>
       <c r="K94" s="20"/>
-      <c r="L94" s="20"/>
+      <c r="L94" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test cases status has been updated
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="419">
   <si>
     <t>Descreption</t>
   </si>
@@ -962,9 +962,6 @@
 3- Click on Register
 4- Fill in the form
 5-Click on Submit button</t>
-  </si>
-  <si>
-    <t>When clicking on submit button, the data entered by user should be sent to the database.</t>
   </si>
   <si>
     <t>Verify that the user info added to the database</t>
@@ -1555,7 +1552,38 @@
     <t>There are no * beside the mandatory fields</t>
   </si>
   <si>
-    <t>Server error page comes up when pressing on submit button</t>
+    <t>When clicking on submit button, the data entered by user should be sent to the database.
+And the user will be redirected to the home page</t>
+  </si>
+  <si>
+    <t>The user has been successfully redirected to the home page</t>
+  </si>
+  <si>
+    <t>The user has been added succesfully to the database</t>
+  </si>
+  <si>
+    <t>The error message displayed successfully</t>
+  </si>
+  <si>
+    <t>The system accepted the username and added it to the database</t>
+  </si>
+  <si>
+    <t>The username has been accepted successfully by the system and added to the database</t>
+  </si>
+  <si>
+    <t>The system refused to proceed while leaving the optional fields empty</t>
+  </si>
+  <si>
+    <t>The system accepted the username although it is already existing</t>
+  </si>
+  <si>
+    <t>The system generated an error message to tell the user that the passwords entered don't match</t>
+  </si>
+  <si>
+    <t>The system refused to proceed and displayed the error message</t>
+  </si>
+  <si>
+    <t>The system  proceeded successfully with submitting the form</t>
   </si>
 </sst>
 </file>
@@ -2029,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72"/>
+    <sheetView tabSelected="1" topLeftCell="D92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2073,7 +2101,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>0</v>
@@ -3317,7 +3345,7 @@
         <v>274</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>212</v>
@@ -3383,7 +3411,7 @@
         <v>274</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>221</v>
@@ -3449,7 +3477,7 @@
         <v>274</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="6" t="s">
@@ -3482,7 +3510,7 @@
         <v>274</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="6" t="s">
@@ -3516,7 +3544,7 @@
         <v>274</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="6" t="s">
@@ -3550,7 +3578,7 @@
         <v>274</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H65" s="6" t="s">
         <v>242</v>
@@ -3616,7 +3644,7 @@
         <v>274</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>266</v>
@@ -3648,7 +3676,7 @@
         <v>274</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>268</v>
@@ -3665,7 +3693,7 @@
     </row>
     <row r="69" spans="1:12" s="5" customFormat="1" ht="26">
       <c r="A69" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -3681,7 +3709,7 @@
     </row>
     <row r="70" spans="1:12" ht="101.5">
       <c r="A70" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>227</v>
@@ -3703,7 +3731,7 @@
         <v>276</v>
       </c>
       <c r="I70" s="20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J70" s="6" t="s">
         <v>277</v>
@@ -3715,7 +3743,7 @@
     </row>
     <row r="71" spans="1:12" ht="72.5">
       <c r="A71" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>227</v>
@@ -3737,7 +3765,7 @@
         <v>281</v>
       </c>
       <c r="I71" s="20" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J71" s="6" t="s">
         <v>277</v>
@@ -3749,7 +3777,7 @@
     </row>
     <row r="72" spans="1:12" ht="101.5">
       <c r="A72" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>282</v>
@@ -3768,7 +3796,7 @@
       </c>
       <c r="G72" s="20"/>
       <c r="H72" s="20" t="s">
-        <v>286</v>
+        <v>408</v>
       </c>
       <c r="I72" s="20" t="s">
         <v>409</v>
@@ -3777,695 +3805,785 @@
         <v>277</v>
       </c>
       <c r="K72" s="20"/>
-      <c r="L72" s="6"/>
+      <c r="L72" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="73" spans="1:12" ht="145">
       <c r="A73" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C73" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="D73" s="20" t="s">
         <v>287</v>
-      </c>
-      <c r="D73" s="20" t="s">
-        <v>288</v>
       </c>
       <c r="E73" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F73" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G73" s="20"/>
       <c r="H73" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="I73" s="20"/>
+        <v>288</v>
+      </c>
+      <c r="I73" s="20" t="s">
+        <v>410</v>
+      </c>
       <c r="J73" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K73" s="20"/>
-      <c r="L73" s="6"/>
+      <c r="L73" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="74" spans="1:12" ht="116">
       <c r="A74" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C74" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D74" s="20" t="s">
         <v>290</v>
-      </c>
-      <c r="D74" s="20" t="s">
-        <v>291</v>
       </c>
       <c r="E74" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G74" s="20"/>
       <c r="H74" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="I74" s="20"/>
+        <v>292</v>
+      </c>
+      <c r="I74" s="20" t="s">
+        <v>411</v>
+      </c>
       <c r="J74" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K74" s="20"/>
-      <c r="L74" s="6"/>
+      <c r="L74" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="75" spans="1:12" ht="116">
       <c r="A75" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C75" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="D75" s="20" t="s">
         <v>294</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>295</v>
       </c>
       <c r="E75" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G75" s="20"/>
       <c r="H75" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="I75" s="20"/>
+        <v>296</v>
+      </c>
+      <c r="I75" s="20" t="s">
+        <v>411</v>
+      </c>
       <c r="J75" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K75" s="20"/>
-      <c r="L75" s="6"/>
+      <c r="L75" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="76" spans="1:12" ht="116">
       <c r="A76" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C76" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="D76" s="20" t="s">
         <v>298</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>299</v>
       </c>
       <c r="E76" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G76" s="20"/>
       <c r="H76" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="I76" s="20"/>
+        <v>300</v>
+      </c>
+      <c r="I76" s="20" t="s">
+        <v>411</v>
+      </c>
       <c r="J76" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K76" s="20"/>
-      <c r="L76" s="6"/>
+      <c r="L76" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="77" spans="1:12" ht="101.5">
       <c r="A77" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C77" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="D77" s="20" t="s">
         <v>302</v>
-      </c>
-      <c r="D77" s="20" t="s">
-        <v>303</v>
       </c>
       <c r="E77" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G77" s="20"/>
       <c r="H77" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="I77" s="20"/>
+        <v>304</v>
+      </c>
+      <c r="I77" s="20" t="s">
+        <v>411</v>
+      </c>
       <c r="J77" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K77" s="20"/>
-      <c r="L77" s="6"/>
+      <c r="L77" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="78" spans="1:12" ht="116">
       <c r="A78" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C78" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="D78" s="20" t="s">
         <v>306</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>307</v>
       </c>
       <c r="E78" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F78" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="G78" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="G78" s="20" t="s">
+      <c r="H78" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="H78" s="20" t="s">
-        <v>310</v>
-      </c>
-      <c r="I78" s="20"/>
+      <c r="I78" s="20" t="s">
+        <v>412</v>
+      </c>
       <c r="J78" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K78" s="20"/>
-      <c r="L78" s="6"/>
+      <c r="L78" s="23" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="79" spans="1:12" ht="87">
       <c r="A79" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C79" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="D79" s="20" t="s">
         <v>311</v>
-      </c>
-      <c r="D79" s="20" t="s">
-        <v>312</v>
       </c>
       <c r="E79" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F79" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="G79" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="G79" s="20" t="s">
-        <v>314</v>
-      </c>
       <c r="H79" s="20" t="s">
-        <v>310</v>
-      </c>
-      <c r="I79" s="20"/>
+        <v>309</v>
+      </c>
+      <c r="I79" s="20" t="s">
+        <v>412</v>
+      </c>
       <c r="J79" s="6"/>
       <c r="K79" s="20"/>
-      <c r="L79" s="6"/>
+      <c r="L79" s="23" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="80" spans="1:12" ht="116">
       <c r="A80" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C80" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="D80" s="20" t="s">
         <v>315</v>
-      </c>
-      <c r="D80" s="20" t="s">
-        <v>316</v>
       </c>
       <c r="E80" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F80" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="G80" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="G80" s="20" t="s">
+      <c r="H80" s="20" t="s">
         <v>318</v>
       </c>
-      <c r="H80" s="20" t="s">
-        <v>319</v>
-      </c>
-      <c r="I80" s="20"/>
+      <c r="I80" s="20" t="s">
+        <v>413</v>
+      </c>
       <c r="J80" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K80" s="20"/>
-      <c r="L80" s="6"/>
+      <c r="L80" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="81" spans="1:12" ht="101.5">
       <c r="A81" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C81" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="D81" s="20" t="s">
         <v>320</v>
-      </c>
-      <c r="D81" s="20" t="s">
-        <v>321</v>
       </c>
       <c r="E81" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G81" s="20"/>
       <c r="H81" s="20" t="s">
-        <v>319</v>
-      </c>
-      <c r="I81" s="20"/>
+        <v>318</v>
+      </c>
+      <c r="I81" s="20" t="s">
+        <v>414</v>
+      </c>
       <c r="J81" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K81" s="20"/>
-      <c r="L81" s="6"/>
+      <c r="L81" s="23" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="82" spans="1:12" ht="116">
       <c r="A82" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C82" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="D82" s="20" t="s">
         <v>323</v>
-      </c>
-      <c r="D82" s="20" t="s">
-        <v>324</v>
       </c>
       <c r="E82" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G82" s="20"/>
       <c r="H82" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="I82" s="20"/>
+        <v>325</v>
+      </c>
+      <c r="I82" s="20" t="s">
+        <v>415</v>
+      </c>
       <c r="J82" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K82" s="20"/>
-      <c r="L82" s="6"/>
+      <c r="L82" s="23" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="83" spans="1:12" ht="145">
       <c r="A83" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C83" s="20" t="s">
+        <v>326</v>
+      </c>
+      <c r="D83" s="20" t="s">
         <v>327</v>
-      </c>
-      <c r="D83" s="20" t="s">
-        <v>328</v>
       </c>
       <c r="E83" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F83" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="G83" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="G83" s="20" t="s">
+      <c r="H83" s="20" t="s">
         <v>330</v>
       </c>
-      <c r="H83" s="20" t="s">
-        <v>331</v>
-      </c>
-      <c r="I83" s="20"/>
+      <c r="I83" s="20" t="s">
+        <v>416</v>
+      </c>
       <c r="J83" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K83" s="20"/>
-      <c r="L83" s="6"/>
+      <c r="L83" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="84" spans="1:12" ht="159.5">
       <c r="A84" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C84" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="D84" s="20" t="s">
         <v>332</v>
-      </c>
-      <c r="D84" s="20" t="s">
-        <v>333</v>
       </c>
       <c r="E84" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F84" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="G84" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="G84" s="20" t="s">
+      <c r="H84" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="H84" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="I84" s="20"/>
+      <c r="I84" s="20" t="s">
+        <v>417</v>
+      </c>
       <c r="J84" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K84" s="20"/>
-      <c r="L84" s="6"/>
+      <c r="L84" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="85" spans="1:12" ht="159.5">
       <c r="A85" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D85" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E85" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F85" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="G85" s="20" t="s">
         <v>338</v>
       </c>
-      <c r="G85" s="20" t="s">
-        <v>339</v>
-      </c>
       <c r="H85" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="I85" s="20"/>
+        <v>335</v>
+      </c>
+      <c r="I85" s="20" t="s">
+        <v>417</v>
+      </c>
       <c r="J85" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K85" s="20"/>
-      <c r="L85" s="6"/>
+      <c r="L85" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="86" spans="1:12" ht="145">
       <c r="A86" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C86" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="D86" s="20" t="s">
         <v>340</v>
-      </c>
-      <c r="D86" s="20" t="s">
-        <v>341</v>
       </c>
       <c r="E86" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F86" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="G86" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="G86" s="20" t="s">
-        <v>343</v>
-      </c>
       <c r="H86" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="I86" s="20"/>
+        <v>335</v>
+      </c>
+      <c r="I86" s="20" t="s">
+        <v>417</v>
+      </c>
       <c r="J86" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K86" s="20"/>
-      <c r="L86" s="6"/>
+      <c r="L86" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="87" spans="1:12" ht="159.5">
       <c r="A87" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C87" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="D87" s="20" t="s">
         <v>344</v>
-      </c>
-      <c r="D87" s="20" t="s">
-        <v>345</v>
       </c>
       <c r="E87" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F87" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="G87" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="G87" s="20" t="s">
-        <v>347</v>
-      </c>
       <c r="H87" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="I87" s="20"/>
+        <v>335</v>
+      </c>
+      <c r="I87" s="20" t="s">
+        <v>417</v>
+      </c>
       <c r="J87" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K87" s="20"/>
-      <c r="L87" s="6"/>
+      <c r="L87" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="88" spans="1:12" ht="159.5">
       <c r="A88" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E88" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F88" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="G88" s="20" t="s">
         <v>349</v>
       </c>
-      <c r="G88" s="20" t="s">
-        <v>350</v>
-      </c>
       <c r="H88" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="I88" s="20"/>
+        <v>335</v>
+      </c>
+      <c r="I88" s="20" t="s">
+        <v>417</v>
+      </c>
       <c r="J88" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K88" s="20"/>
-      <c r="L88" s="6"/>
+      <c r="L88" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="89" spans="1:12" ht="145">
       <c r="A89" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C89" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="D89" s="20" t="s">
         <v>351</v>
-      </c>
-      <c r="D89" s="20" t="s">
-        <v>352</v>
       </c>
       <c r="E89" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F89" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="G89" s="20" t="s">
         <v>353</v>
       </c>
-      <c r="G89" s="20" t="s">
-        <v>354</v>
-      </c>
       <c r="H89" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="I89" s="20"/>
+        <v>335</v>
+      </c>
+      <c r="I89" s="20" t="s">
+        <v>417</v>
+      </c>
       <c r="J89" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K89" s="20"/>
-      <c r="L89" s="6"/>
+      <c r="L89" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="90" spans="1:12" ht="130.5">
       <c r="A90" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C90" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="D90" s="20" t="s">
         <v>355</v>
-      </c>
-      <c r="D90" s="20" t="s">
-        <v>356</v>
       </c>
       <c r="E90" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F90" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="G90" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="G90" s="20" t="s">
+      <c r="H90" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="H90" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="I90" s="20"/>
+      <c r="I90" s="20" t="s">
+        <v>418</v>
+      </c>
       <c r="J90" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K90" s="20"/>
-      <c r="L90" s="6"/>
+      <c r="L90" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="91" spans="1:12" ht="145">
       <c r="A91" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C91" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="D91" s="20" t="s">
         <v>360</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>361</v>
       </c>
       <c r="E91" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F91" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="G91" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="G91" s="20" t="s">
+      <c r="H91" s="20" t="s">
         <v>363</v>
       </c>
-      <c r="H91" s="20" t="s">
-        <v>364</v>
-      </c>
-      <c r="I91" s="20"/>
+      <c r="I91" s="20" t="s">
+        <v>417</v>
+      </c>
       <c r="J91" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K91" s="20"/>
-      <c r="L91" s="6"/>
+      <c r="L91" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="92" spans="1:12" ht="145">
       <c r="A92" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D92" s="20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E92" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H92" s="20" t="s">
-        <v>364</v>
-      </c>
-      <c r="I92" s="20"/>
+        <v>363</v>
+      </c>
+      <c r="I92" s="20" t="s">
+        <v>417</v>
+      </c>
       <c r="J92" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K92" s="20"/>
-      <c r="L92" s="6"/>
+      <c r="L92" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="93" spans="1:12" ht="145">
       <c r="A93" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D93" s="20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E93" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F93" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G93" s="20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H93" s="20" t="s">
-        <v>364</v>
-      </c>
-      <c r="I93" s="20"/>
+        <v>363</v>
+      </c>
+      <c r="I93" s="20" t="s">
+        <v>417</v>
+      </c>
       <c r="J93" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K93" s="20"/>
-      <c r="L93" s="6"/>
+      <c r="L93" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="94" spans="1:12" ht="145">
       <c r="A94" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D94" s="20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E94" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F94" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G94" s="20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H94" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="I94" s="20"/>
+        <v>358</v>
+      </c>
+      <c r="I94" s="20" t="s">
+        <v>418</v>
+      </c>
       <c r="J94" s="6" t="s">
         <v>277</v>
       </c>
       <c r="K94" s="20"/>
-      <c r="L94" s="6"/>
+      <c r="L94" s="22" t="s">
+        <v>258</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>